<commit_message>
exe and Changes.py Added
</commit_message>
<xml_diff>
--- a/resultados.xlsx
+++ b/resultados.xlsx
@@ -536,7 +536,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>COMP-ABC-100</t>
+          <t>COMP-THC-6106</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -586,7 +586,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>COMP-ABC-100</t>
+          <t>COMP-THC-6106</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -638,7 +638,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>COMP-ABC-100</t>
+          <t>COMP-THC-6106</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -688,7 +688,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>ABC-100</t>
+          <t>THC-6106</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -738,7 +738,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>ABC-101</t>
+          <t>THC-6107</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -788,7 +788,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>ABC-102</t>
+          <t>THC-6108</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -838,7 +838,7 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>COMP-ABC-103</t>
+          <t>COMP-THC-6109</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -888,7 +888,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>COMP-ABC-103</t>
+          <t>COMP-THC-6109</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -940,7 +940,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>COMP-ABC-103</t>
+          <t>COMP-THC-6109</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -990,7 +990,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>ABC-103</t>
+          <t>THC-6109</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -1040,7 +1040,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>ABC-104</t>
+          <t>THC-6110</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1090,7 +1090,7 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>ABC-105</t>
+          <t>THC-6111</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
@@ -1140,7 +1140,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>COMP-ABC-106</t>
+          <t>COMP-THC-6112</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1190,7 +1190,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>COMP-ABC-106</t>
+          <t>COMP-THC-6112</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1242,7 +1242,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>COMP-ABC-106</t>
+          <t>COMP-THC-6112</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1292,7 +1292,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>ABC-106</t>
+          <t>THC-6112</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1342,7 +1342,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>ABC-107</t>
+          <t>THC-6113</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
@@ -1392,7 +1392,7 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>ABC-108</t>
+          <t>THC-6114</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -1442,7 +1442,7 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>ABC-108</t>
+          <t>THC-6114</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -1492,7 +1492,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>ABC-108</t>
+          <t>THC-6114</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -1540,7 +1540,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>COMP-ABC-108</t>
+          <t>COMP-THC-6114</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -1592,7 +1592,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>COMP-ABC-109</t>
+          <t>COMP-THC-6115</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -1642,7 +1642,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>ABC-110</t>
+          <t>THC-6116</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -1692,7 +1692,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>COMP-ABC-111</t>
+          <t>COMP-THC-6117</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -1746,7 +1746,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>ABC-111</t>
+          <t>THC-6117</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -1794,7 +1794,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>COMP-ABC-111</t>
+          <t>COMP-THC-6117</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -1844,7 +1844,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>COMP-ABC-111</t>
+          <t>COMP-THC-6117</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -1894,7 +1894,7 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>ABC-112</t>
+          <t>THC-6118</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -1942,7 +1942,7 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>COMP-ABC-112</t>
+          <t>COMP-THC-6118</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
@@ -1992,7 +1992,7 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>ABC-112</t>
+          <t>THC-6118</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -2046,7 +2046,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>COMP-ABC-112</t>
+          <t>COMP-THC-6118</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -2096,7 +2096,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>COMP-ABC-113</t>
+          <t>COMP-THC-6119</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -2148,7 +2148,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>ABC-113</t>
+          <t>THC-6119</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -2200,7 +2200,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>COMP-ABC-113</t>
+          <t>COMP-THC-6119</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -2252,7 +2252,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>COMP-ABC-113</t>
+          <t>COMP-THC-6119</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -2308,7 +2308,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>ABC-113</t>
+          <t>THC-6119</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -2358,7 +2358,7 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>COMP-ABC-113</t>
+          <t>COMP-THC-6119</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
@@ -2410,7 +2410,7 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>COMP-ABC-113</t>
+          <t>COMP-THC-6119</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
@@ -2462,7 +2462,7 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>ABC-113</t>
+          <t>THC-6119</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
@@ -2512,7 +2512,7 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>ABC-114</t>
+          <t>THC-6120</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>COMP-ABC-115</t>
+          <t>COMP-THC-6121</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
@@ -2610,7 +2610,7 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>COMP-ABC-115</t>
+          <t>COMP-THC-6121</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
@@ -2660,7 +2660,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>ABC-116</t>
+          <t>THC-6122</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
@@ -2714,7 +2714,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>ABC-116</t>
+          <t>THC-6122</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">

</xml_diff>